<commit_message>
fixed code for evaluating models and wrote script for generating loo run models
</commit_message>
<xml_diff>
--- a/CLIP Final Model Results.xlsx
+++ b/CLIP Final Model Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Portable\Documents\GitHub\CMPUT624_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14BAAAC5-6BAC-4C36-ABFD-E5337D4E175D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401A5F63-43B4-4D90-A3D8-6C9055B9ED8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
   <si>
     <t>Text Format</t>
   </si>
@@ -100,6 +100,27 @@
   </si>
   <si>
     <t>slurm-42667107</t>
+  </si>
+  <si>
+    <t>LOO Runs (within subject)</t>
+  </si>
+  <si>
+    <t>slurm-42682826</t>
+  </si>
+  <si>
+    <t>slurm-42682904</t>
+  </si>
+  <si>
+    <t>slurm-42682907</t>
+  </si>
+  <si>
+    <t>slurm-42682908</t>
+  </si>
+  <si>
+    <t>slurm-42682914</t>
+  </si>
+  <si>
+    <t>slurm-42682920</t>
   </si>
 </sst>
 </file>
@@ -426,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,6 +537,9 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
       <c r="E4">
         <v>2</v>
       </c>
@@ -569,61 +593,100 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14">
-        <v>10</v>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B19" t="s">
         <v>11</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C19" t="s">
         <v>12</v>
       </c>
-      <c r="D17">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>23</v>
+      <c r="D19">
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>